<commit_message>
Refactored entProcessor to ent_processing
</commit_message>
<xml_diff>
--- a/data/test/test_gpt3F_entsR.xlsx
+++ b/data/test/test_gpt3F_entsR.xlsx
@@ -514,7 +514,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>[{"factor": ["thioredoxin concentration", "serum"], "outcome": ["in-hospital major adverse event"]}, {"factor": ["glasgow coma scale score", "admission"], "outcome": ["in-hospital major adverse event"]}]</t>
+          <t>[{"factor": ["thioredoxin concentration", "serum"], "outcome": ["in-hospital major adverse event"]}, {"factor": ["admission", "glasgow coma scale score"], "outcome": ["in-hospital major adverse event"]}]</t>
         </is>
       </c>
     </row>
@@ -673,7 +673,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>[{"factor": ["glasgow coma scale score"], "outcome": ["glasgow outcome scale", "gos"]}, {"factor": ["artificial ventilation"], "outcome": ["mortality rate"]}, {"factor": ["monitoring", "intracranial"], "outcome": ["outcome", "long-term", "good"]}]</t>
+          <t>[{"factor": ["glasgow coma scale score"], "outcome": ["glasgow outcome scale", "gos"]}, {"factor": ["artificial ventilation"], "outcome": ["mortality rate"]}, {"factor": ["intracranial", "monitoring"], "outcome": ["long-term", "outcome", "good"]}]</t>
         </is>
       </c>
     </row>
@@ -726,7 +726,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>[{"factor": ["impact", "calculator", "prognosis"], "outcome": ["patient", "elderly", "severe", "outcome", "tbi"]}, {"factor": ["expect risk", "fatal", "outcome"], "outcome": ["risk", "conservative treatment"]}, {"factor": ["outcome", "unfavorable", "predict risk"], "outcome": ["actual", "rate", "risk", "outcome", "unfavorable", "predict"]}]</t>
+          <t>[{"factor": ["impact", "calculator", "prognosis"], "outcome": ["elderly", "tbi", "severe", "outcome", "patient"]}, {"factor": ["expect risk", "outcome", "fatal"], "outcome": ["risk", "conservative treatment"]}, {"factor": ["unfavorable", "outcome", "predict risk"], "outcome": ["risk", "outcome", "rate", "actual", "predict", "unfavorable"]}]</t>
         </is>
       </c>
     </row>
@@ -779,7 +779,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>[{"factor": ["time post-tbi"], "outcome": ["percentage", "cognitive functionality gain"]}, {"factor": ["cognitive function", "admission"], "outcome": ["percentage", "cognitive functionality gain"]}]</t>
+          <t>[{"factor": ["time post-tbi"], "outcome": ["percentage", "cognitive functionality gain"]}, {"factor": ["admission", "cognitive function"], "outcome": ["percentage", "cognitive functionality gain"]}]</t>
         </is>
       </c>
     </row>
@@ -832,7 +832,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>[{"factor": ["compute tomography", "ct"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["marshall and rotterdam scoring system"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["basal cistern absence"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["positive midline shift"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["hemorrhagic mass volume"], "outcome": ["death", "patient", "tbi"]}, {"factor": ["intraventricular", "subarachnoid hemorrhage"], "outcome": ["death", "patient", "tbi"]}]</t>
+          <t>[{"factor": ["ct", "compute tomography"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["marshall and rotterdam scoring system"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["basal cistern absence"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["positive midline shift"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["hemorrhagic mass volume"], "outcome": ["patient", "tbi", "death"]}, {"factor": ["intraventricular", "subarachnoid hemorrhage"], "outcome": ["patient", "tbi", "death"]}]</t>
         </is>
       </c>
     </row>
@@ -885,7 +885,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>[{"factor": ["apache ii"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}, {"factor": ["sap ii"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}, {"factor": ["sofa"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}, {"factor": ["age"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}, {"factor": ["glasgow coma scale"], "outcome": ["icu-treated", "mortality", "patient", "tbi", "six-month"]}]</t>
+          <t>[{"factor": ["apache ii"], "outcome": ["icu-treated", "tbi", "six-month", "patient", "mortality"]}, {"factor": ["sap ii"], "outcome": ["icu-treated", "tbi", "six-month", "patient", "mortality"]}, {"factor": ["sofa"], "outcome": ["icu-treated", "tbi", "six-month", "patient", "mortality"]}, {"factor": ["age"], "outcome": ["icu-treated", "tbi", "six-month", "patient", "mortality"]}, {"factor": ["glasgow coma scale"], "outcome": ["icu-treated", "tbi", "six-month", "patient", "mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -938,7 +938,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>[{"factor": ["v/c ratio"], "outcome": ["drs", "gos score", "lcf score"]}]</t>
+          <t>[{"factor": ["v/c ratio"], "outcome": ["gos score", "lcf score", "drs"]}]</t>
         </is>
       </c>
     </row>
@@ -991,7 +991,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>[{"factor": ["timp-1 level", "serum"], "outcome": ["tbi", "patient", "severe", "mortality"]}]</t>
+          <t>[{"factor": ["timp-1 level", "serum"], "outcome": ["patient", "tbi", "mortality", "severe"]}]</t>
         </is>
       </c>
     </row>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>[{"factor": ["evidence", "contusion", "mri"], "outcome": ["glasgow outcome scale-extended", "gos-e"]}, {"factor": ["roi", "severely", "fa", "reduce"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["age"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}, {"factor": ["roi", "severely", "fa", "reduce"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}]</t>
+          <t>[{"factor": ["contusion", "mri", "evidence"], "outcome": ["glasgow outcome scale-extended", "gos-e"]}, {"factor": ["reduce", "roi", "severely", "fa"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["age"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}, {"factor": ["reduce", "roi", "severely", "fa"], "outcome": ["gos-e"]}, {"factor": ["neuropsychiatric history"], "outcome": ["gos-e"]}, {"factor": ["year of"], "outcome": ["gos-e"]}]</t>
         </is>
       </c>
     </row>
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>[{"factor": ["preinjury", "depressive symptom"], "outcome": ["affective/behavioral", "physical problem", "cognitive", "health-related quality-of-life"]}]</t>
+          <t>[{"factor": ["depressive symptom", "preinjury"], "outcome": ["health-related quality-of-life", "physical problem", "cognitive", "affective/behavioral"]}]</t>
         </is>
       </c>
     </row>
@@ -1309,7 +1309,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>[{"factor": ["concentration", "cerebrospinal fluid", "csf", "amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["concentration", "plasma", "amyloid-beta1-42 (abeta42)"], "outcome": ["mortality"]}, {"factor": ["abeta42", "change", "concentration", "csf"], "outcome": ["neurological status"]}]</t>
+          <t>[{"factor": ["csf", "cerebrospinal fluid", "amyloid-beta1-42 (abeta42)", "concentration"], "outcome": ["mortality"]}, {"factor": ["amyloid-beta1-42 (abeta42)", "concentration", "plasma"], "outcome": ["mortality"]}, {"factor": ["change", "csf", "concentration", "abeta42"], "outcome": ["neurological status"]}]</t>
         </is>
       </c>
     </row>
@@ -1362,7 +1362,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>[{"factor": ["plasminogen activator receptor", "supar", "soluble", "urokinase"], "outcome": ["traumatic brain injury", "tbi"]}, {"factor": ["glasgow coma scale", "score"], "outcome": ["severity", "tbi"]}, {"factor": ["d-dimer"], "outcome": ["tbi", "patient", "mortality"]}]</t>
+          <t>[{"factor": ["plasminogen activator receptor", "urokinase", "soluble", "supar"], "outcome": ["tbi", "traumatic brain injury"]}, {"factor": ["score", "glasgow coma scale"], "outcome": ["severity", "tbi"]}, {"factor": ["d-dimer"], "outcome": ["patient", "tbi", "mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -1415,7 +1415,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>[{"factor": ["motor score", "gcs"], "outcome": ["month", "mortality"]}, {"factor": ["age"], "outcome": ["month", "mortality"]}, {"factor": ["sex"], "outcome": ["month", "mortality"]}, {"factor": ["injury", "mechanism"], "outcome": ["month", "mortality"]}, {"factor": ["glasgow coma scale"], "outcome": ["month", "mortality"]}, {"factor": ["intubation"], "outcome": ["month", "mortality"]}, {"factor": ["pupil"], "outcome": ["month", "mortality"]}, {"factor": ["systolic blood pressure"], "outcome": ["month", "mortality"]}, {"factor": ["respiratory rate"], "outcome": ["month", "mortality"]}, {"factor": ["body temperature"], "outcome": ["month", "mortality"]}, {"factor": ["arterial", "ph"], "outcome": ["month", "mortality"]}, {"factor": ["arterial partial pressure", "carbon dioxide"], "outcome": ["month", "mortality"]}, {"factor": ["arterial partial pressure"], "outcome": ["month", "mortality"]}, {"factor": ["serum sodium"], "outcome": ["month", "mortality"]}, {"factor": ["serum potassium"], "outcome": ["month", "mortality"]}, {"factor": ["serum chloride"], "outcome": ["month", "mortality"]}, {"factor": ["serum calcium"], "outcome": ["month", "mortality"]}, {"factor": ["serum glucose"], "outcome": ["month", "mortality"]}, {"factor": ["urea nitrogen"], "outcome": ["month", "mortality"]}, {"factor": ["creatinine"], "outcome": ["month", "mortality"]}, {"factor": ["ratio", "international"], "outcome": ["month", "mortality"]}]</t>
+          <t>[{"factor": ["motor score", "gcs"], "outcome": ["mortality", "month"]}, {"factor": ["age"], "outcome": ["mortality", "month"]}, {"factor": ["sex"], "outcome": ["mortality", "month"]}, {"factor": ["mechanism", "injury"], "outcome": ["mortality", "month"]}, {"factor": ["glasgow coma scale"], "outcome": ["mortality", "month"]}, {"factor": ["intubation"], "outcome": ["mortality", "month"]}, {"factor": ["pupil"], "outcome": ["mortality", "month"]}, {"factor": ["systolic blood pressure"], "outcome": ["mortality", "month"]}, {"factor": ["respiratory rate"], "outcome": ["mortality", "month"]}, {"factor": ["body temperature"], "outcome": ["mortality", "month"]}, {"factor": ["ph", "arterial"], "outcome": ["mortality", "month"]}, {"factor": ["arterial partial pressure", "carbon dioxide"], "outcome": ["mortality", "month"]}, {"factor": ["arterial partial pressure"], "outcome": ["mortality", "month"]}, {"factor": ["serum sodium"], "outcome": ["mortality", "month"]}, {"factor": ["serum potassium"], "outcome": ["mortality", "month"]}, {"factor": ["serum chloride"], "outcome": ["mortality", "month"]}, {"factor": ["serum calcium"], "outcome": ["mortality", "month"]}, {"factor": ["serum glucose"], "outcome": ["mortality", "month"]}, {"factor": ["urea nitrogen"], "outcome": ["mortality", "month"]}, {"factor": ["creatinine"], "outcome": ["mortality", "month"]}, {"factor": ["international", "ratio"], "outcome": ["mortality", "month"]}]</t>
         </is>
       </c>
     </row>
@@ -1468,7 +1468,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>[{"factor": ["aptt"], "outcome": ["deterioration", "surgery"]}, {"factor": ["fdp"], "outcome": ["deterioration", "surgery"]}, {"factor": ["d-dimer"], "outcome": ["deterioration", "surgery"]}]</t>
+          <t>[{"factor": ["aptt"], "outcome": ["surgery", "deterioration"]}, {"factor": ["fdp"], "outcome": ["surgery", "deterioration"]}, {"factor": ["d-dimer"], "outcome": ["surgery", "deterioration"]}]</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>[{"factor": ["cct", "central conduction time"], "outcome": ["clinical outcome", "long-term"]}, {"factor": ["latency"], "outcome": ["clinical outcome", "long-term"]}]</t>
+          <t>[{"factor": ["central conduction time", "cct"], "outcome": ["long-term", "clinical outcome"]}, {"factor": ["latency"], "outcome": ["long-term", "clinical outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>[{"factor": ["tsp-1"], "outcome": ["outcome", "unfavorable", "1-week", "mortality"]}]</t>
+          <t>[{"factor": ["tsp-1"], "outcome": ["unfavorable", "1-week", "mortality", "outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -1733,7 +1733,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>[{"factor": ["brain-derived neurotrophic factor (bdnf)", "plasma level"], "outcome": ["icu", "mortality", "patient", "severe", "intensive care unit", "tbi"]}]</t>
+          <t>[{"factor": ["plasma level", "brain-derived neurotrophic factor (bdnf)"], "outcome": ["tbi", "severe", "patient", "intensive care unit", "icu", "mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -1786,7 +1786,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>[{"factor": ["crash-ct model"], "outcome": ["death", "days"]}, {"factor": ["age"], "outcome": ["patient", "performance", "model", "older"]}, {"factor": ["glasgow coma scale score"], "outcome": ["discrimination", "model"]}, {"factor": ["hosmer-lemeshow p value"], "outcome": ["calibration", "model"]}]</t>
+          <t>[{"factor": ["crash-ct model"], "outcome": ["days", "death"]}, {"factor": ["age"], "outcome": ["older", "patient", "model", "performance"]}, {"factor": ["glasgow coma scale score"], "outcome": ["discrimination", "model"]}, {"factor": ["hosmer-lemeshow p value"], "outcome": ["model", "calibration"]}]</t>
         </is>
       </c>
     </row>
@@ -1839,7 +1839,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>[{"factor": ["time to death"], "outcome": ["withdrawal", "life-sustaining", "therapy"]}, {"factor": ["glasgow coma scale", "score"], "outcome": ["mortality"]}, {"factor": ["score", "ais", "head abbreviate injury scale"], "outcome": ["mortality"]}, {"factor": ["comorbiditie", "multiple"], "outcome": ["mortality"]}, {"factor": ["subarachnoid hemorrhage", "traumatic"], "outcome": ["mortality"]}, {"factor": ["intracerebral mass lesion"], "outcome": ["mortality"]}, {"factor": ["brainstem lesion"], "outcome": ["mortality"]}, {"factor": ["absent", "sign of compress", "basal cistern"], "outcome": ["mortality"]}]</t>
+          <t>[{"factor": ["time to death"], "outcome": ["withdrawal", "life-sustaining", "therapy"]}, {"factor": ["score", "glasgow coma scale"], "outcome": ["mortality"]}, {"factor": ["ais", "score", "head abbreviate injury scale"], "outcome": ["mortality"]}, {"factor": ["multiple", "comorbiditie"], "outcome": ["mortality"]}, {"factor": ["traumatic", "subarachnoid hemorrhage"], "outcome": ["mortality"]}, {"factor": ["intracerebral mass lesion"], "outcome": ["mortality"]}, {"factor": ["brainstem lesion"], "outcome": ["mortality"]}, {"factor": ["absent", "sign of compress", "basal cistern"], "outcome": ["mortality"]}]</t>
         </is>
       </c>
     </row>
@@ -1892,7 +1892,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>[{"factor": ["core model"], "outcome": ["mortality"]}, {"factor": ["extend model"], "outcome": ["mortality"]}, {"factor": ["lab model"], "outcome": ["mortality"]}, {"factor": ["core model"], "outcome": ["outcome", "unfavorable"]}, {"factor": ["extend model"], "outcome": ["outcome", "unfavorable"]}, {"factor": ["lab model"], "outcome": ["outcome", "unfavorable"]}]</t>
+          <t>[{"factor": ["core model"], "outcome": ["mortality"]}, {"factor": ["extend model"], "outcome": ["mortality"]}, {"factor": ["lab model"], "outcome": ["mortality"]}, {"factor": ["core model"], "outcome": ["unfavorable", "outcome"]}, {"factor": ["extend model"], "outcome": ["unfavorable", "outcome"]}, {"factor": ["lab model"], "outcome": ["unfavorable", "outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -1945,7 +1945,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>[{"factor": ["glasgow coma scale", "score"], "outcome": ["outcome", "unfavorable", "1-week", "mortality"]}]</t>
+          <t>[{"factor": ["score", "glasgow coma scale"], "outcome": ["unfavorable", "1-week", "mortality", "outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -1998,7 +1998,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>[{"factor": ["gcs", "glasgow coma scale"], "outcome": ["severity", "tbi"]}, {"factor": ["pta", "duration", "post-traumatic amnesia"], "outcome": ["olfactory problem", "tbi"]}]</t>
+          <t>[{"factor": ["gcs", "glasgow coma scale"], "outcome": ["severity", "tbi"]}, {"factor": ["duration", "pta", "post-traumatic amnesia"], "outcome": ["tbi", "olfactory problem"]}]</t>
         </is>
       </c>
     </row>
@@ -2051,7 +2051,7 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>[{"factor": ["level", "il-6"], "outcome": ["septic", "development"]}, {"factor": ["c-reactive protein level"], "outcome": ["multiple organ dysfunction", "development"]}]</t>
+          <t>[{"factor": ["level", "il-6"], "outcome": ["development", "septic"]}, {"factor": ["c-reactive protein level"], "outcome": ["development", "multiple organ dysfunction"]}]</t>
         </is>
       </c>
     </row>
@@ -2104,7 +2104,7 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>[{"factor": ["rotterdam"], "outcome": ["death", "hospital discharge", "weeks"]}, {"factor": ["age"], "outcome": ["death", "hospital discharge", "weeks"]}, {"factor": ["sex"], "outcome": ["death", "hospital discharge", "weeks"]}, {"factor": ["glasgow coma scale score"], "outcome": ["death", "hospital discharge", "weeks"]}]</t>
+          <t>[{"factor": ["rotterdam"], "outcome": ["hospital discharge", "death", "weeks"]}, {"factor": ["age"], "outcome": ["hospital discharge", "death", "weeks"]}, {"factor": ["sex"], "outcome": ["hospital discharge", "death", "weeks"]}, {"factor": ["glasgow coma scale score"], "outcome": ["hospital discharge", "death", "weeks"]}]</t>
         </is>
       </c>
     </row>
@@ -2157,7 +2157,7 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>[{"factor": ["glucose", "serum", "admission", "level of"], "outcome": ["outcome", "traumatic brain injury", "patient", "severe"]}]</t>
+          <t>[{"factor": ["admission", "serum", "glucose", "level of"], "outcome": ["patient", "outcome", "traumatic brain injury", "severe"]}]</t>
         </is>
       </c>
     </row>
@@ -2210,7 +2210,7 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>[{"factor": ["csf"], "outcome": ["month", "gos score"]}, {"factor": ["sfas"], "outcome": ["month", "gos score"]}, {"factor": ["il-10"], "outcome": ["month", "gos score"]}, {"factor": ["il-6"], "outcome": ["month", "gos score"]}, {"factor": ["svcam-1"], "outcome": ["month", "gos score"]}, {"factor": ["il-5"], "outcome": ["month", "gos score"]}, {"factor": ["il-8"], "outcome": ["month", "gos score"]}, {"factor": ["pc1"], "outcome": ["month", "gos score"]}, {"factor": [], "outcome": ["month", "gos score"]}, {"factor": [], "outcome": ["month", "gos score"]}]</t>
+          <t>[{"factor": ["csf"], "outcome": ["gos score", "month"]}, {"factor": ["sfas"], "outcome": ["gos score", "month"]}, {"factor": ["il-10"], "outcome": ["gos score", "month"]}, {"factor": ["il-6"], "outcome": ["gos score", "month"]}, {"factor": ["svcam-1"], "outcome": ["gos score", "month"]}, {"factor": ["il-5"], "outcome": ["gos score", "month"]}, {"factor": ["il-8"], "outcome": ["gos score", "month"]}, {"factor": ["pc1"], "outcome": ["gos score", "month"]}, {"factor": [], "outcome": ["gos score", "month"]}, {"factor": [], "outcome": ["gos score", "month"]}]</t>
         </is>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>[{"factor": ["age"], "outcome": ["poor outcome"]}, {"factor": ["glasgow coma scale"], "outcome": ["poor outcome"]}, {"factor": ["injury", "severity score"], "outcome": ["poor outcome"]}, {"factor": ["ais", "head"], "outcome": ["poor outcome"]}]</t>
+          <t>[{"factor": ["age"], "outcome": ["poor outcome"]}, {"factor": ["glasgow coma scale"], "outcome": ["poor outcome"]}, {"factor": ["severity score", "injury"], "outcome": ["poor outcome"]}, {"factor": ["ais", "head"], "outcome": ["poor outcome"]}]</t>
         </is>
       </c>
     </row>
@@ -2316,7 +2316,7 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>[{"factor": ["il-6"], "outcome": ["year", "favorable", "gos"]}, {"factor": ["pg"], "outcome": ["year", "favorable", "gos"]}, {"factor": ["gfap"], "outcome": ["unfavorable", "year", "score", "gos"]}, {"factor": ["pg"], "outcome": ["survival status", "year"]}, {"factor": ["gfap"], "outcome": ["survival status", "year"]}, {"factor": ["il-6"], "outcome": ["survival status", "year"]}]</t>
+          <t>[{"factor": ["il-6"], "outcome": ["year", "gos", "favorable"]}, {"factor": ["pg"], "outcome": ["year", "gos", "favorable"]}, {"factor": ["gfap"], "outcome": ["year", "unfavorable", "score", "gos"]}, {"factor": ["pg"], "outcome": ["survival status", "year"]}, {"factor": ["gfap"], "outcome": ["survival status", "year"]}, {"factor": ["il-6"], "outcome": ["survival status", "year"]}]</t>
         </is>
       </c>
     </row>
@@ -2369,7 +2369,7 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>[{"factor": ["acute"], "outcome": ["drs", "score"]}, {"factor": ["subacute", "fa"], "outcome": ["drs", "score"]}]</t>
+          <t>[{"factor": ["acute"], "outcome": ["score", "drs"]}, {"factor": ["subacute", "fa"], "outcome": ["score", "drs"]}]</t>
         </is>
       </c>
     </row>
@@ -2422,7 +2422,7 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>[{"factor": ["glasgow coma scale"], "outcome": ["mortality"]}, {"factor": ["mechanical ventilation"], "outcome": ["neurological"]}, {"factor": ["blood transfusion"], "outcome": ["neurological"]}, {"factor": ["neurosurgical intervention"], "outcome": ["neurological"]}, {"factor": ["concomitant", "injury"], "outcome": ["complication", "non-neurological"]}]</t>
+          <t>[{"factor": ["glasgow coma scale"], "outcome": ["mortality"]}, {"factor": ["mechanical ventilation"], "outcome": ["neurological"]}, {"factor": ["blood transfusion"], "outcome": ["neurological"]}, {"factor": ["neurosurgical intervention"], "outcome": ["neurological"]}, {"factor": ["injury", "concomitant"], "outcome": ["non-neurological", "complication"]}]</t>
         </is>
       </c>
     </row>

</xml_diff>